<commit_message>
Update User Data Again--
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="27945" windowHeight="11925"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="工作表1" sheetId="1" r:id="rId4"/>
+    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -31,64 +47,926 @@
     <t>Iwak</t>
   </si>
   <si>
-    <t>KItten</t>
+    <t>Kitten</t>
   </si>
   <si>
-    <t>O57ADKey</t>
+    <t>O57AD</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Thus</t>
+  </si>
+  <si>
+    <t>Testing3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="9">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+    </tableStyle>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -278,20 +1156,24 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6" outlineLevelCol="2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" customHeight="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -302,7 +1184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" customHeight="1" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -310,10 +1192,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" customHeight="1" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -321,10 +1203,10 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" customHeight="1" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -332,10 +1214,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" customHeight="1" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -343,10 +1225,33 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>5.0</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>333333</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>